<commit_message>
Update Insert User data  file
</commit_message>
<xml_diff>
--- a/UserProfileImportTemplate.xlsx
+++ b/UserProfileImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TERM9(FTL)\SEP490\AptCare_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07969679-623C-47A1-9AD9-F4FF66C5CB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D40AB8D-DABD-444E-BADB-5418E02B5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FCE59F89-A2A7-4AA2-B0DD-734913F4A020}"/>
   </bookViews>
@@ -238,9 +238,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -580,7 +582,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:I13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,11 +596,11 @@
     <col min="9" max="9" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -627,7 +629,7 @@
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -636,7 +638,7 @@
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="4">
@@ -648,7 +650,7 @@
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -656,7 +658,7 @@
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -665,7 +667,7 @@
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="4">
@@ -677,7 +679,7 @@
       <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -685,7 +687,7 @@
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -694,7 +696,7 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="4">
@@ -706,7 +708,7 @@
       <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -714,7 +716,7 @@
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -723,7 +725,7 @@
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="2"/>
@@ -733,7 +735,7 @@
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -741,7 +743,7 @@
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -750,7 +752,7 @@
       <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="4">
@@ -762,7 +764,7 @@
       <c r="H6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="7" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MailSender Setting, UserManagement(Update, Insert by excel file, Create account for new User(No data), Create User Data), TokenGeneration for login
</commit_message>
<xml_diff>
--- a/UserProfileImportTemplate.xlsx
+++ b/UserProfileImportTemplate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TERM9(FTL)\SEP490\AptCare_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D40AB8D-DABD-444E-BADB-5418E02B5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF0977-77E3-415D-8D86-D3C7C063C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{FCE59F89-A2A7-4AA2-B0DD-734913F4A020}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{FCE59F89-A2A7-4AA2-B0DD-734913F4A020}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="UserApartments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>A-101</t>
   </si>
@@ -135,9 +136,6 @@
   </si>
   <si>
     <t>0623812111111111111111</t>
-  </si>
-  <si>
-    <t>'0623812111111111111111</t>
   </si>
   <si>
     <t>RelationshipToOwnerType</t>
@@ -579,24 +577,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232F5AB1-2BFC-47B5-A10B-ADD59311AD68}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="5" width="38.28515625" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" customWidth="1"/>
-    <col min="8" max="8" width="41.42578125" customWidth="1"/>
-    <col min="9" max="9" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -615,17 +610,8 @@
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -644,17 +630,8 @@
       <c r="F2" s="4">
         <v>29221</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -673,17 +650,8 @@
       <c r="F3" s="4">
         <v>29952</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -702,70 +670,25 @@
       <c r="F4" s="4">
         <v>38353</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F5" s="4">
         <v>32874</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -773,9 +696,113 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{464415CB-B866-48FA-9F89-77BAB62879CC}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{E35613FC-CFDD-4571-BF89-0E2CAE4CCB0E}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{EB8519CD-898B-4001-89E2-33B651B03922}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{B41618B5-3245-4F02-BFC7-49623C3FCF13}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{0A1893C3-8D91-499E-B643-447DD13B3BFB}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{0A1893C3-8D91-499E-B643-447DD13B3BFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C44318C-5C8E-44C4-B5C8-9E90D7CD2CDF}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>